<commit_message>
Es werden nur die Kreise überhalb dem Mittelpunkt der Flasche gezählt
</commit_message>
<xml_diff>
--- a/Features_Test.xlsx
+++ b/Features_Test.xlsx
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>0.3846153846153846</v>
@@ -471,7 +471,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>0.7401129943502824</v>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>0.362962962962963</v>
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
         <v>0.7450271247739603</v>
@@ -519,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>0.3897058823529412</v>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
         <v>0.5011286681715575</v>
@@ -551,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0.459016393442623</v>
@@ -567,7 +567,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
         <v>0.4986807387862797</v>
@@ -583,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>0.5386313465783664</v>
@@ -599,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0.5845070422535211</v>
@@ -615,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0.8557919621749409</v>
@@ -631,7 +631,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
         <v>0.8767123287671232</v>
@@ -647,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0.9430051813471503</v>
@@ -663,7 +663,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>0.7982646420824295</v>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
         <v>0.4818181818181818</v>
@@ -695,7 +695,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0.4759725400457666</v>
@@ -711,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
         <v>0.4515418502202643</v>
@@ -727,7 +727,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
         <v>0.4701834862385321</v>
@@ -743,7 +743,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>0.4730679156908665</v>
@@ -759,7 +759,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" t="n">
         <v>0.9530916844349681</v>
@@ -775,7 +775,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
         <v>1.032679738562092</v>
@@ -791,7 +791,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
         <v>1.074324324324324</v>
@@ -807,7 +807,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
         <v>1.115044247787611</v>
@@ -855,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
         <v>0.7136563876651982</v>
@@ -871,7 +871,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
         <v>0.7314814814814815</v>
@@ -887,7 +887,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C29" t="n">
         <v>0.7431818181818182</v>
@@ -903,7 +903,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0.9079903147699758</v>
@@ -919,7 +919,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
         <v>0.509719222462203</v>
@@ -935,7 +935,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C32" t="n">
         <v>0.8340909090909091</v>
@@ -951,7 +951,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C33" t="n">
         <v>0.676056338028169</v>
@@ -967,7 +967,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
         <v>0.4775828460038986</v>
@@ -983,7 +983,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
         <v>0.5357142857142857</v>
@@ -999,7 +999,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
         <v>0.6697459584295612</v>
@@ -1015,7 +1015,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C37" t="n">
         <v>0.7074340527577938</v>
@@ -1047,7 +1047,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C39" t="n">
         <v>0.5531496062992126</v>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C40" t="n">
         <v>0.5609243697478992</v>
@@ -1079,7 +1079,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
         <v>0.5991471215351812</v>
@@ -1095,7 +1095,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C42" t="n">
         <v>0.6850220264317181</v>
@@ -1111,7 +1111,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C43" t="n">
         <v>0.5204460966542751</v>
@@ -1127,7 +1127,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" t="n">
         <v>0.3903345724907063</v>
@@ -1143,7 +1143,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C45" t="n">
         <v>0.392156862745098</v>
@@ -1159,7 +1159,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
         <v>0.4427767354596623</v>
@@ -1175,7 +1175,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C47" t="n">
         <v>0.4091743119266055</v>
@@ -1191,7 +1191,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
         <v>0.6743801652892562</v>
@@ -1207,7 +1207,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
         <v>0.3871559633027523</v>
@@ -1223,7 +1223,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C50" t="n">
         <v>0.4220532319391635</v>
@@ -1239,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C51" t="n">
         <v>0.4296028880866426</v>
@@ -1255,7 +1255,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C52" t="n">
         <v>0.3844936708860759</v>
@@ -1271,7 +1271,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C53" t="n">
         <v>0.4088586030664395</v>
@@ -1287,7 +1287,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C54" t="n">
         <v>0.8782608695652174</v>
@@ -1303,7 +1303,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C55" t="n">
         <v>0.44874715261959</v>
@@ -1319,7 +1319,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
         <v>0.44874715261959</v>
@@ -1335,7 +1335,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
         <v>0.4475524475524476</v>
@@ -1351,7 +1351,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C58" t="n">
         <v>0.4568764568764569</v>
@@ -1367,7 +1367,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C59" t="n">
         <v>0.5346320346320347</v>
@@ -1383,7 +1383,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C60" t="n">
         <v>0.5186813186813187</v>
@@ -1399,7 +1399,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C61" t="n">
         <v>0.4309978768577495</v>
@@ -1415,7 +1415,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C62" t="n">
         <v>1.269565217391304</v>
@@ -1431,7 +1431,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C63" t="n">
         <v>0.6502732240437158</v>
@@ -1447,7 +1447,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
         <v>0.4547325102880658</v>
@@ -1463,7 +1463,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
         <v>0.5145413870246085</v>
@@ -1479,7 +1479,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C66" t="n">
         <v>0.8088803088803089</v>
@@ -1495,7 +1495,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
         <v>0.5137254901960784</v>
@@ -1511,7 +1511,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C68" t="n">
         <v>0.6572052401746725</v>
@@ -1527,7 +1527,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
         <v>0.788546255506608</v>
@@ -1543,7 +1543,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
         <v>0.6943907156673114</v>
@@ -1559,7 +1559,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" t="n">
         <v>0.693069306930693</v>
@@ -1575,7 +1575,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C72" t="n">
         <v>0.6549707602339181</v>
@@ -1591,7 +1591,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" t="n">
         <v>1.011415525114155</v>
@@ -1607,7 +1607,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C74" t="n">
         <v>0.8560885608856088</v>
@@ -1623,7 +1623,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C75" t="n">
         <v>0.8420107719928187</v>
@@ -1639,7 +1639,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C76" t="n">
         <v>0.4029126213592233</v>
@@ -1655,7 +1655,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C77" t="n">
         <v>0.4129263913824057</v>
@@ -1671,7 +1671,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C78" t="n">
         <v>0.8451400329489291</v>
@@ -1687,7 +1687,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C79" t="n">
         <v>0.9311377245508982</v>
@@ -1703,7 +1703,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C80" t="n">
         <v>0.8615916955017301</v>
@@ -1719,7 +1719,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
         <v>1.120300751879699</v>
@@ -1751,7 +1751,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C83" t="n">
         <v>0.9246987951807228</v>
@@ -1767,7 +1767,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C84" t="n">
         <v>1.176923076923077</v>
@@ -1783,7 +1783,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C85" t="n">
         <v>0.8736462093862816</v>
@@ -1799,7 +1799,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C86" t="n">
         <v>0.9664179104477612</v>
@@ -1815,7 +1815,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C87" t="n">
         <v>1.158088235294118</v>
@@ -1831,7 +1831,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
         <v>0.9724137931034482</v>
@@ -1847,7 +1847,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C89" t="n">
         <v>1.060070671378092</v>
@@ -1863,7 +1863,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C90" t="n">
         <v>1.094736842105263</v>
@@ -1879,7 +1879,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C91" t="n">
         <v>0.8654545454545455</v>
@@ -1895,7 +1895,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C92" t="n">
         <v>0.9498069498069498</v>
@@ -1911,7 +1911,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C93" t="n">
         <v>1.019417475728155</v>
@@ -1927,7 +1927,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
         <v>1.27536231884058</v>
@@ -1943,7 +1943,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C95" t="n">
         <v>0.51183970856102</v>
@@ -1959,7 +1959,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C96" t="n">
         <v>0.7184265010351967</v>
@@ -1975,7 +1975,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
         <v>0.6290672451193059</v>
@@ -1991,7 +1991,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C98" t="n">
         <v>0.5625</v>
@@ -2007,7 +2007,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C99" t="n">
         <v>0.5273833671399595</v>
@@ -2023,7 +2023,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C100" t="n">
         <v>0.6557692307692308</v>

</xml_diff>

<commit_message>
Ecken werden in der oberen Hälfte des Rechtecks detektiert
</commit_message>
<xml_diff>
--- a/Features_Test.xlsx
+++ b/Features_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Anzahl Ecken</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Labels</t>
         </is>
       </c>
@@ -460,7 +465,10 @@
       <c r="C2" t="n">
         <v>0.3846153846153846</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -476,7 +484,10 @@
       <c r="C3" t="n">
         <v>0.7401129943502824</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -492,7 +503,10 @@
       <c r="C4" t="n">
         <v>0.362962962962963</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -508,7 +522,10 @@
       <c r="C5" t="n">
         <v>0.7450271247739603</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -524,7 +541,10 @@
       <c r="C6" t="n">
         <v>0.3897058823529412</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -540,7 +560,10 @@
       <c r="C7" t="n">
         <v>0.5011286681715575</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -556,7 +579,10 @@
       <c r="C8" t="n">
         <v>0.459016393442623</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -572,7 +598,10 @@
       <c r="C9" t="n">
         <v>0.4986807387862797</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -588,7 +617,10 @@
       <c r="C10" t="n">
         <v>0.5386313465783664</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -604,7 +636,10 @@
       <c r="C11" t="n">
         <v>0.5845070422535211</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -620,7 +655,10 @@
       <c r="C12" t="n">
         <v>0.8557919621749409</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -636,7 +674,10 @@
       <c r="C13" t="n">
         <v>0.8767123287671232</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -652,7 +693,10 @@
       <c r="C14" t="n">
         <v>0.9430051813471503</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -668,7 +712,10 @@
       <c r="C15" t="n">
         <v>0.7982646420824295</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -684,7 +731,10 @@
       <c r="C16" t="n">
         <v>0.4818181818181818</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -700,7 +750,10 @@
       <c r="C17" t="n">
         <v>0.4759725400457666</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -716,7 +769,10 @@
       <c r="C18" t="n">
         <v>0.4515418502202643</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -732,7 +788,10 @@
       <c r="C19" t="n">
         <v>0.4701834862385321</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D19" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -748,7 +807,10 @@
       <c r="C20" t="n">
         <v>0.4730679156908665</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -764,7 +826,10 @@
       <c r="C21" t="n">
         <v>0.9530916844349681</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -780,7 +845,10 @@
       <c r="C22" t="n">
         <v>1.032679738562092</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -796,7 +864,10 @@
       <c r="C23" t="n">
         <v>1.074324324324324</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -812,7 +883,10 @@
       <c r="C24" t="n">
         <v>1.115044247787611</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -828,7 +902,10 @@
       <c r="C25" t="n">
         <v>1.130820399113082</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -844,7 +921,10 @@
       <c r="C26" t="n">
         <v>0.6422018348623854</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="D26" t="n">
+        <v>7</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -860,7 +940,10 @@
       <c r="C27" t="n">
         <v>0.7136563876651982</v>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="D27" t="n">
+        <v>11</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -876,7 +959,10 @@
       <c r="C28" t="n">
         <v>0.7314814814814815</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -892,7 +978,10 @@
       <c r="C29" t="n">
         <v>0.7431818181818182</v>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="D29" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -908,7 +997,10 @@
       <c r="C30" t="n">
         <v>0.9079903147699758</v>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="D30" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -924,7 +1016,10 @@
       <c r="C31" t="n">
         <v>0.509719222462203</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -940,7 +1035,10 @@
       <c r="C32" t="n">
         <v>0.8340909090909091</v>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" t="n">
+        <v>9</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -956,7 +1054,10 @@
       <c r="C33" t="n">
         <v>0.676056338028169</v>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="D33" t="n">
+        <v>8</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -972,7 +1073,10 @@
       <c r="C34" t="n">
         <v>0.4775828460038986</v>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D34" t="n">
+        <v>7</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -988,7 +1092,10 @@
       <c r="C35" t="n">
         <v>0.5357142857142857</v>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="D35" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1004,7 +1111,10 @@
       <c r="C36" t="n">
         <v>0.6697459584295612</v>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1020,7 +1130,10 @@
       <c r="C37" t="n">
         <v>0.7074340527577938</v>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="D37" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1036,7 +1149,10 @@
       <c r="C38" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1052,7 +1168,10 @@
       <c r="C39" t="n">
         <v>0.5531496062992126</v>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="D39" t="n">
+        <v>7</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1068,7 +1187,10 @@
       <c r="C40" t="n">
         <v>0.5609243697478992</v>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1084,7 +1206,10 @@
       <c r="C41" t="n">
         <v>0.5991471215351812</v>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1100,7 +1225,10 @@
       <c r="C42" t="n">
         <v>0.6850220264317181</v>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="D42" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1116,7 +1244,10 @@
       <c r="C43" t="n">
         <v>0.5204460966542751</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1132,7 +1263,10 @@
       <c r="C44" t="n">
         <v>0.3903345724907063</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D44" t="n">
+        <v>5</v>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1148,7 +1282,10 @@
       <c r="C45" t="n">
         <v>0.392156862745098</v>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1164,7 +1301,10 @@
       <c r="C46" t="n">
         <v>0.4427767354596623</v>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="D46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1180,7 +1320,10 @@
       <c r="C47" t="n">
         <v>0.4091743119266055</v>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="D47" t="n">
+        <v>4</v>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1196,7 +1339,10 @@
       <c r="C48" t="n">
         <v>0.6743801652892562</v>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="D48" t="n">
+        <v>7</v>
+      </c>
+      <c r="E48" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1212,7 +1358,10 @@
       <c r="C49" t="n">
         <v>0.3871559633027523</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1228,7 +1377,10 @@
       <c r="C50" t="n">
         <v>0.4220532319391635</v>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="D50" t="n">
+        <v>6</v>
+      </c>
+      <c r="E50" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1244,7 +1396,10 @@
       <c r="C51" t="n">
         <v>0.4296028880866426</v>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1260,7 +1415,10 @@
       <c r="C52" t="n">
         <v>0.3844936708860759</v>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1276,7 +1434,10 @@
       <c r="C53" t="n">
         <v>0.4088586030664395</v>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="D53" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1292,7 +1453,10 @@
       <c r="C54" t="n">
         <v>0.8782608695652174</v>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="D54" t="n">
+        <v>5</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1308,7 +1472,10 @@
       <c r="C55" t="n">
         <v>0.44874715261959</v>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D55" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1324,7 +1491,10 @@
       <c r="C56" t="n">
         <v>0.44874715261959</v>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="D56" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1340,7 +1510,10 @@
       <c r="C57" t="n">
         <v>0.4475524475524476</v>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1356,7 +1529,10 @@
       <c r="C58" t="n">
         <v>0.4568764568764569</v>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="D58" t="n">
+        <v>2</v>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1372,7 +1548,10 @@
       <c r="C59" t="n">
         <v>0.5346320346320347</v>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="D59" t="n">
+        <v>6</v>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1388,7 +1567,10 @@
       <c r="C60" t="n">
         <v>0.5186813186813187</v>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="D60" t="n">
+        <v>5</v>
+      </c>
+      <c r="E60" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1404,7 +1586,10 @@
       <c r="C61" t="n">
         <v>0.4309978768577495</v>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="D61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1420,7 +1605,10 @@
       <c r="C62" t="n">
         <v>1.269565217391304</v>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="D62" t="n">
+        <v>6</v>
+      </c>
+      <c r="E62" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1436,7 +1624,10 @@
       <c r="C63" t="n">
         <v>0.6502732240437158</v>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D63" t="n">
+        <v>8</v>
+      </c>
+      <c r="E63" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1452,7 +1643,10 @@
       <c r="C64" t="n">
         <v>0.4547325102880658</v>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="D64" t="n">
+        <v>5</v>
+      </c>
+      <c r="E64" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1468,7 +1662,10 @@
       <c r="C65" t="n">
         <v>0.5145413870246085</v>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="D65" t="n">
+        <v>3</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1484,7 +1681,10 @@
       <c r="C66" t="n">
         <v>0.8088803088803089</v>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="D66" t="n">
+        <v>8</v>
+      </c>
+      <c r="E66" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1500,7 +1700,10 @@
       <c r="C67" t="n">
         <v>0.5137254901960784</v>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="D67" t="n">
+        <v>4</v>
+      </c>
+      <c r="E67" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1516,7 +1719,10 @@
       <c r="C68" t="n">
         <v>0.6572052401746725</v>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D68" t="n">
+        <v>2</v>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1532,7 +1738,10 @@
       <c r="C69" t="n">
         <v>0.788546255506608</v>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1548,7 +1757,10 @@
       <c r="C70" t="n">
         <v>0.6943907156673114</v>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1564,7 +1776,10 @@
       <c r="C71" t="n">
         <v>0.693069306930693</v>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D71" t="n">
+        <v>5</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1580,7 +1795,10 @@
       <c r="C72" t="n">
         <v>0.6549707602339181</v>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D72" t="n">
+        <v>9</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1596,7 +1814,10 @@
       <c r="C73" t="n">
         <v>1.011415525114155</v>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1612,7 +1833,10 @@
       <c r="C74" t="n">
         <v>0.8560885608856088</v>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1628,7 +1852,10 @@
       <c r="C75" t="n">
         <v>0.8420107719928187</v>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1644,7 +1871,10 @@
       <c r="C76" t="n">
         <v>0.4029126213592233</v>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D76" t="n">
+        <v>2</v>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1660,7 +1890,10 @@
       <c r="C77" t="n">
         <v>0.4129263913824057</v>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D77" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1676,7 +1909,10 @@
       <c r="C78" t="n">
         <v>0.8451400329489291</v>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="D78" t="n">
+        <v>6</v>
+      </c>
+      <c r="E78" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1692,7 +1928,10 @@
       <c r="C79" t="n">
         <v>0.9311377245508982</v>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="D79" t="n">
+        <v>2</v>
+      </c>
+      <c r="E79" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1708,7 +1947,10 @@
       <c r="C80" t="n">
         <v>0.8615916955017301</v>
       </c>
-      <c r="D80" t="inlineStr">
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1724,7 +1966,10 @@
       <c r="C81" t="n">
         <v>1.120300751879699</v>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1740,7 +1985,10 @@
       <c r="C82" t="n">
         <v>0.8113207547169812</v>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1756,7 +2004,10 @@
       <c r="C83" t="n">
         <v>0.9246987951807228</v>
       </c>
-      <c r="D83" t="inlineStr">
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1772,7 +2023,10 @@
       <c r="C84" t="n">
         <v>1.176923076923077</v>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="D84" t="n">
+        <v>5</v>
+      </c>
+      <c r="E84" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1788,7 +2042,10 @@
       <c r="C85" t="n">
         <v>0.8736462093862816</v>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1804,7 +2061,10 @@
       <c r="C86" t="n">
         <v>0.9664179104477612</v>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1820,7 +2080,10 @@
       <c r="C87" t="n">
         <v>1.158088235294118</v>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="D87" t="n">
+        <v>7</v>
+      </c>
+      <c r="E87" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1836,7 +2099,10 @@
       <c r="C88" t="n">
         <v>0.9724137931034482</v>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="D88" t="n">
+        <v>2</v>
+      </c>
+      <c r="E88" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1852,7 +2118,10 @@
       <c r="C89" t="n">
         <v>1.060070671378092</v>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D89" t="n">
+        <v>2</v>
+      </c>
+      <c r="E89" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1868,7 +2137,10 @@
       <c r="C90" t="n">
         <v>1.094736842105263</v>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1884,7 +2156,10 @@
       <c r="C91" t="n">
         <v>0.8654545454545455</v>
       </c>
-      <c r="D91" t="inlineStr">
+      <c r="D91" t="n">
+        <v>6</v>
+      </c>
+      <c r="E91" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1900,7 +2175,10 @@
       <c r="C92" t="n">
         <v>0.9498069498069498</v>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="D92" t="n">
+        <v>2</v>
+      </c>
+      <c r="E92" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1916,7 +2194,10 @@
       <c r="C93" t="n">
         <v>1.019417475728155</v>
       </c>
-      <c r="D93" t="inlineStr">
+      <c r="D93" t="n">
+        <v>2</v>
+      </c>
+      <c r="E93" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1932,7 +2213,10 @@
       <c r="C94" t="n">
         <v>1.27536231884058</v>
       </c>
-      <c r="D94" t="inlineStr">
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+      <c r="E94" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1948,7 +2232,10 @@
       <c r="C95" t="n">
         <v>0.51183970856102</v>
       </c>
-      <c r="D95" t="inlineStr">
+      <c r="D95" t="n">
+        <v>4</v>
+      </c>
+      <c r="E95" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1964,7 +2251,10 @@
       <c r="C96" t="n">
         <v>0.7184265010351967</v>
       </c>
-      <c r="D96" t="inlineStr">
+      <c r="D96" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1980,7 +2270,10 @@
       <c r="C97" t="n">
         <v>0.6290672451193059</v>
       </c>
-      <c r="D97" t="inlineStr">
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1996,7 +2289,10 @@
       <c r="C98" t="n">
         <v>0.5625</v>
       </c>
-      <c r="D98" t="inlineStr">
+      <c r="D98" t="n">
+        <v>3</v>
+      </c>
+      <c r="E98" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2012,7 +2308,10 @@
       <c r="C99" t="n">
         <v>0.5273833671399595</v>
       </c>
-      <c r="D99" t="inlineStr">
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2028,7 +2327,10 @@
       <c r="C100" t="n">
         <v>0.6557692307692308</v>
       </c>
-      <c r="D100" t="inlineStr">
+      <c r="D100" t="n">
+        <v>4</v>
+      </c>
+      <c r="E100" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>

</xml_diff>

<commit_message>
Keypoints deteketieren (SIFT) hinzugefügt
</commit_message>
<xml_diff>
--- a/Features_Test.xlsx
+++ b/Features_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Anzahl Keypoints</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Labels</t>
         </is>
       </c>
@@ -468,7 +473,10 @@
       <c r="D2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>197</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -487,7 +495,10 @@
       <c r="D3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>204</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -506,7 +517,10 @@
       <c r="D4" t="n">
         <v>2</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>138</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -525,7 +539,10 @@
       <c r="D5" t="n">
         <v>6</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="n">
+        <v>218</v>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -544,7 +561,10 @@
       <c r="D6" t="n">
         <v>3</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>121</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -563,7 +583,10 @@
       <c r="D7" t="n">
         <v>4</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="n">
+        <v>279</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -582,7 +605,10 @@
       <c r="D8" t="n">
         <v>3</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="n">
+        <v>184</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -601,7 +627,10 @@
       <c r="D9" t="n">
         <v>4</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="n">
+        <v>144</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -620,7 +649,10 @@
       <c r="D10" t="n">
         <v>5</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" t="n">
+        <v>294</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -639,7 +671,10 @@
       <c r="D11" t="n">
         <v>1</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" t="n">
+        <v>225</v>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -658,7 +693,10 @@
       <c r="D12" t="n">
         <v>6</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>220</v>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -677,7 +715,10 @@
       <c r="D13" t="n">
         <v>1</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" t="n">
+        <v>271</v>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -696,7 +737,10 @@
       <c r="D14" t="n">
         <v>6</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="n">
+        <v>235</v>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -715,7 +759,10 @@
       <c r="D15" t="n">
         <v>8</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="n">
+        <v>243</v>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -734,7 +781,10 @@
       <c r="D16" t="n">
         <v>3</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="n">
+        <v>122</v>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -753,7 +803,10 @@
       <c r="D17" t="n">
         <v>3</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="n">
+        <v>118</v>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -772,7 +825,10 @@
       <c r="D18" t="n">
         <v>4</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" t="n">
+        <v>163</v>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -791,7 +847,10 @@
       <c r="D19" t="n">
         <v>3</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" t="n">
+        <v>106</v>
+      </c>
+      <c r="F19" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -810,7 +869,10 @@
       <c r="D20" t="n">
         <v>3</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" t="n">
+        <v>95</v>
+      </c>
+      <c r="F20" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -829,7 +891,10 @@
       <c r="D21" t="n">
         <v>3</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E21" t="n">
+        <v>260</v>
+      </c>
+      <c r="F21" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -848,7 +913,10 @@
       <c r="D22" t="n">
         <v>4</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" t="n">
+        <v>224</v>
+      </c>
+      <c r="F22" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -867,7 +935,10 @@
       <c r="D23" t="n">
         <v>1</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E23" t="n">
+        <v>183</v>
+      </c>
+      <c r="F23" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -886,7 +957,10 @@
       <c r="D24" t="n">
         <v>5</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E24" t="n">
+        <v>174</v>
+      </c>
+      <c r="F24" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -905,7 +979,10 @@
       <c r="D25" t="n">
         <v>2</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E25" t="n">
+        <v>184</v>
+      </c>
+      <c r="F25" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -924,7 +1001,10 @@
       <c r="D26" t="n">
         <v>7</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E26" t="n">
+        <v>131</v>
+      </c>
+      <c r="F26" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -943,7 +1023,10 @@
       <c r="D27" t="n">
         <v>11</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E27" t="n">
+        <v>289</v>
+      </c>
+      <c r="F27" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -962,7 +1045,10 @@
       <c r="D28" t="n">
         <v>3</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E28" t="n">
+        <v>220</v>
+      </c>
+      <c r="F28" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -981,7 +1067,10 @@
       <c r="D29" t="n">
         <v>8</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E29" t="n">
+        <v>230</v>
+      </c>
+      <c r="F29" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1000,7 +1089,10 @@
       <c r="D30" t="n">
         <v>4</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="n">
+        <v>234</v>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1019,7 +1111,10 @@
       <c r="D31" t="n">
         <v>4</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E31" t="n">
+        <v>236</v>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1038,7 +1133,10 @@
       <c r="D32" t="n">
         <v>9</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="n">
+        <v>244</v>
+      </c>
+      <c r="F32" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1057,7 +1155,10 @@
       <c r="D33" t="n">
         <v>8</v>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" t="n">
+        <v>125</v>
+      </c>
+      <c r="F33" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1076,7 +1177,10 @@
       <c r="D34" t="n">
         <v>7</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E34" t="n">
+        <v>93</v>
+      </c>
+      <c r="F34" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1095,7 +1199,10 @@
       <c r="D35" t="n">
         <v>6</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="n">
+        <v>360</v>
+      </c>
+      <c r="F35" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1114,7 +1221,10 @@
       <c r="D36" t="n">
         <v>1</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="n">
+        <v>260</v>
+      </c>
+      <c r="F36" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1133,7 +1243,10 @@
       <c r="D37" t="n">
         <v>3</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E37" t="n">
+        <v>158</v>
+      </c>
+      <c r="F37" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1152,7 +1265,10 @@
       <c r="D38" t="n">
         <v>4</v>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" t="n">
+        <v>130</v>
+      </c>
+      <c r="F38" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1171,7 +1287,10 @@
       <c r="D39" t="n">
         <v>7</v>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" t="n">
+        <v>103</v>
+      </c>
+      <c r="F39" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1190,7 +1309,10 @@
       <c r="D40" t="n">
         <v>2</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" t="n">
+        <v>118</v>
+      </c>
+      <c r="F40" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1209,7 +1331,10 @@
       <c r="D41" t="n">
         <v>5</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E41" t="n">
+        <v>126</v>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1228,7 +1353,10 @@
       <c r="D42" t="n">
         <v>3</v>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E42" t="n">
+        <v>151</v>
+      </c>
+      <c r="F42" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1247,7 +1375,10 @@
       <c r="D43" t="n">
         <v>1</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E43" t="n">
+        <v>367</v>
+      </c>
+      <c r="F43" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1266,7 +1397,10 @@
       <c r="D44" t="n">
         <v>5</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E44" t="n">
+        <v>266</v>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1285,7 +1419,10 @@
       <c r="D45" t="n">
         <v>2</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E45" t="n">
+        <v>188</v>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1304,7 +1441,10 @@
       <c r="D46" t="n">
         <v>4</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="n">
+        <v>141</v>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1323,7 +1463,10 @@
       <c r="D47" t="n">
         <v>4</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E47" t="n">
+        <v>111</v>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1342,7 +1485,10 @@
       <c r="D48" t="n">
         <v>7</v>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E48" t="n">
+        <v>131</v>
+      </c>
+      <c r="F48" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1361,7 +1507,10 @@
       <c r="D49" t="n">
         <v>1</v>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E49" t="n">
+        <v>98</v>
+      </c>
+      <c r="F49" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1380,7 +1529,10 @@
       <c r="D50" t="n">
         <v>6</v>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E50" t="n">
+        <v>138</v>
+      </c>
+      <c r="F50" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1399,7 +1551,10 @@
       <c r="D51" t="n">
         <v>1</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E51" t="n">
+        <v>154</v>
+      </c>
+      <c r="F51" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1418,7 +1573,10 @@
       <c r="D52" t="n">
         <v>1</v>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E52" t="n">
+        <v>224</v>
+      </c>
+      <c r="F52" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1437,7 +1595,10 @@
       <c r="D53" t="n">
         <v>4</v>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E53" t="n">
+        <v>273</v>
+      </c>
+      <c r="F53" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1456,7 +1617,10 @@
       <c r="D54" t="n">
         <v>5</v>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E54" t="n">
+        <v>301</v>
+      </c>
+      <c r="F54" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1475,7 +1639,10 @@
       <c r="D55" t="n">
         <v>3</v>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E55" t="n">
+        <v>239</v>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1494,7 +1661,10 @@
       <c r="D56" t="n">
         <v>3</v>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E56" t="n">
+        <v>216</v>
+      </c>
+      <c r="F56" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1513,7 +1683,10 @@
       <c r="D57" t="n">
         <v>1</v>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E57" t="n">
+        <v>154</v>
+      </c>
+      <c r="F57" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1532,7 +1705,10 @@
       <c r="D58" t="n">
         <v>2</v>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E58" t="n">
+        <v>107</v>
+      </c>
+      <c r="F58" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1551,7 +1727,10 @@
       <c r="D59" t="n">
         <v>6</v>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E59" t="n">
+        <v>219</v>
+      </c>
+      <c r="F59" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1570,7 +1749,10 @@
       <c r="D60" t="n">
         <v>5</v>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E60" t="n">
+        <v>151</v>
+      </c>
+      <c r="F60" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1589,7 +1771,10 @@
       <c r="D61" t="n">
         <v>4</v>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E61" t="n">
+        <v>151</v>
+      </c>
+      <c r="F61" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1608,7 +1793,10 @@
       <c r="D62" t="n">
         <v>6</v>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E62" t="n">
+        <v>299</v>
+      </c>
+      <c r="F62" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1627,7 +1815,10 @@
       <c r="D63" t="n">
         <v>8</v>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E63" t="n">
+        <v>250</v>
+      </c>
+      <c r="F63" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1646,7 +1837,10 @@
       <c r="D64" t="n">
         <v>5</v>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="E64" t="n">
+        <v>214</v>
+      </c>
+      <c r="F64" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1665,7 +1859,10 @@
       <c r="D65" t="n">
         <v>3</v>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E65" t="n">
+        <v>132</v>
+      </c>
+      <c r="F65" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1684,7 +1881,10 @@
       <c r="D66" t="n">
         <v>8</v>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E66" t="n">
+        <v>128</v>
+      </c>
+      <c r="F66" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1703,7 +1903,10 @@
       <c r="D67" t="n">
         <v>4</v>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E67" t="n">
+        <v>152</v>
+      </c>
+      <c r="F67" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1722,7 +1925,10 @@
       <c r="D68" t="n">
         <v>2</v>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E68" t="n">
+        <v>240</v>
+      </c>
+      <c r="F68" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1741,7 +1947,10 @@
       <c r="D69" t="n">
         <v>1</v>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E69" t="n">
+        <v>321</v>
+      </c>
+      <c r="F69" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1760,7 +1969,10 @@
       <c r="D70" t="n">
         <v>1</v>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E70" t="n">
+        <v>229</v>
+      </c>
+      <c r="F70" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1779,7 +1991,10 @@
       <c r="D71" t="n">
         <v>5</v>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E71" t="n">
+        <v>248</v>
+      </c>
+      <c r="F71" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1798,7 +2013,10 @@
       <c r="D72" t="n">
         <v>9</v>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E72" t="n">
+        <v>213</v>
+      </c>
+      <c r="F72" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1817,7 +2035,10 @@
       <c r="D73" t="n">
         <v>2</v>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E73" t="n">
+        <v>262</v>
+      </c>
+      <c r="F73" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1836,7 +2057,10 @@
       <c r="D74" t="n">
         <v>1</v>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E74" t="n">
+        <v>258</v>
+      </c>
+      <c r="F74" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1855,7 +2079,10 @@
       <c r="D75" t="n">
         <v>1</v>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E75" t="n">
+        <v>239</v>
+      </c>
+      <c r="F75" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1874,7 +2101,10 @@
       <c r="D76" t="n">
         <v>2</v>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E76" t="n">
+        <v>125</v>
+      </c>
+      <c r="F76" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1893,7 +2123,10 @@
       <c r="D77" t="n">
         <v>2</v>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E77" t="n">
+        <v>96</v>
+      </c>
+      <c r="F77" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1912,7 +2145,10 @@
       <c r="D78" t="n">
         <v>6</v>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E78" t="n">
+        <v>159</v>
+      </c>
+      <c r="F78" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1931,7 +2167,10 @@
       <c r="D79" t="n">
         <v>2</v>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E79" t="n">
+        <v>136</v>
+      </c>
+      <c r="F79" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1950,7 +2189,10 @@
       <c r="D80" t="n">
         <v>0</v>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="E80" t="n">
+        <v>94</v>
+      </c>
+      <c r="F80" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1969,7 +2211,10 @@
       <c r="D81" t="n">
         <v>0</v>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E81" t="n">
+        <v>84</v>
+      </c>
+      <c r="F81" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -1988,7 +2233,10 @@
       <c r="D82" t="n">
         <v>1</v>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="E82" t="n">
+        <v>108</v>
+      </c>
+      <c r="F82" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2007,7 +2255,10 @@
       <c r="D83" t="n">
         <v>1</v>
       </c>
-      <c r="E83" t="inlineStr">
+      <c r="E83" t="n">
+        <v>182</v>
+      </c>
+      <c r="F83" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2026,7 +2277,10 @@
       <c r="D84" t="n">
         <v>5</v>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E84" t="n">
+        <v>77</v>
+      </c>
+      <c r="F84" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2045,7 +2299,10 @@
       <c r="D85" t="n">
         <v>0</v>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E85" t="n">
+        <v>145</v>
+      </c>
+      <c r="F85" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2064,7 +2321,10 @@
       <c r="D86" t="n">
         <v>1</v>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E86" t="n">
+        <v>139</v>
+      </c>
+      <c r="F86" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2083,7 +2343,10 @@
       <c r="D87" t="n">
         <v>7</v>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E87" t="n">
+        <v>112</v>
+      </c>
+      <c r="F87" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2102,7 +2365,10 @@
       <c r="D88" t="n">
         <v>2</v>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="E88" t="n">
+        <v>148</v>
+      </c>
+      <c r="F88" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2121,7 +2387,10 @@
       <c r="D89" t="n">
         <v>2</v>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="E89" t="n">
+        <v>111</v>
+      </c>
+      <c r="F89" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2140,7 +2409,10 @@
       <c r="D90" t="n">
         <v>1</v>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E90" t="n">
+        <v>74</v>
+      </c>
+      <c r="F90" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2159,7 +2431,10 @@
       <c r="D91" t="n">
         <v>6</v>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E91" t="n">
+        <v>58</v>
+      </c>
+      <c r="F91" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2178,7 +2453,10 @@
       <c r="D92" t="n">
         <v>2</v>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E92" t="n">
+        <v>26</v>
+      </c>
+      <c r="F92" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2197,7 +2475,10 @@
       <c r="D93" t="n">
         <v>2</v>
       </c>
-      <c r="E93" t="inlineStr">
+      <c r="E93" t="n">
+        <v>117</v>
+      </c>
+      <c r="F93" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2216,7 +2497,10 @@
       <c r="D94" t="n">
         <v>2</v>
       </c>
-      <c r="E94" t="inlineStr">
+      <c r="E94" t="n">
+        <v>38</v>
+      </c>
+      <c r="F94" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2235,7 +2519,10 @@
       <c r="D95" t="n">
         <v>4</v>
       </c>
-      <c r="E95" t="inlineStr">
+      <c r="E95" t="n">
+        <v>151</v>
+      </c>
+      <c r="F95" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2254,7 +2541,10 @@
       <c r="D96" t="n">
         <v>1</v>
       </c>
-      <c r="E96" t="inlineStr">
+      <c r="E96" t="n">
+        <v>93</v>
+      </c>
+      <c r="F96" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2273,7 +2563,10 @@
       <c r="D97" t="n">
         <v>1</v>
       </c>
-      <c r="E97" t="inlineStr">
+      <c r="E97" t="n">
+        <v>76</v>
+      </c>
+      <c r="F97" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2292,7 +2585,10 @@
       <c r="D98" t="n">
         <v>3</v>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E98" t="n">
+        <v>75</v>
+      </c>
+      <c r="F98" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2311,7 +2607,10 @@
       <c r="D99" t="n">
         <v>1</v>
       </c>
-      <c r="E99" t="inlineStr">
+      <c r="E99" t="n">
+        <v>87</v>
+      </c>
+      <c r="F99" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2330,7 +2629,10 @@
       <c r="D100" t="n">
         <v>4</v>
       </c>
-      <c r="E100" t="inlineStr">
+      <c r="E100" t="n">
+        <v>157</v>
+      </c>
+      <c r="F100" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>

</xml_diff>

<commit_message>
Liniendetektion in ImagePreprocessing eingebaut Testfunktion für Histogramm eingebaut
</commit_message>
<xml_diff>
--- a/Features_Test.xlsx
+++ b/Features_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Anzahl Linien</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Labels</t>
         </is>
       </c>
@@ -476,7 +481,10 @@
       <c r="E2" t="n">
         <v>197</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -498,7 +506,10 @@
       <c r="E3" t="n">
         <v>204</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -520,7 +531,10 @@
       <c r="E4" t="n">
         <v>138</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -542,7 +556,10 @@
       <c r="E5" t="n">
         <v>218</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -564,7 +581,10 @@
       <c r="E6" t="n">
         <v>121</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -586,7 +606,10 @@
       <c r="E7" t="n">
         <v>279</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -608,7 +631,10 @@
       <c r="E8" t="n">
         <v>184</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -630,7 +656,10 @@
       <c r="E9" t="n">
         <v>144</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -652,7 +681,10 @@
       <c r="E10" t="n">
         <v>294</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -674,7 +706,10 @@
       <c r="E11" t="n">
         <v>225</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>11</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -696,7 +731,10 @@
       <c r="E12" t="n">
         <v>220</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>11</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -718,7 +756,10 @@
       <c r="E13" t="n">
         <v>271</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -740,7 +781,10 @@
       <c r="E14" t="n">
         <v>235</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -762,7 +806,10 @@
       <c r="E15" t="n">
         <v>243</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>9</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -784,7 +831,10 @@
       <c r="E16" t="n">
         <v>122</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -806,7 +856,10 @@
       <c r="E17" t="n">
         <v>118</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -828,7 +881,10 @@
       <c r="E18" t="n">
         <v>163</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -850,7 +906,10 @@
       <c r="E19" t="n">
         <v>106</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -872,7 +931,10 @@
       <c r="E20" t="n">
         <v>95</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -894,7 +956,10 @@
       <c r="E21" t="n">
         <v>260</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -916,7 +981,10 @@
       <c r="E22" t="n">
         <v>224</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>14</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -938,7 +1006,10 @@
       <c r="E23" t="n">
         <v>183</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="n">
+        <v>12</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -960,7 +1031,10 @@
       <c r="E24" t="n">
         <v>174</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="n">
+        <v>10</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -982,7 +1056,10 @@
       <c r="E25" t="n">
         <v>184</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="n">
+        <v>11</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1004,7 +1081,10 @@
       <c r="E26" t="n">
         <v>131</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1026,7 +1106,10 @@
       <c r="E27" t="n">
         <v>289</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1048,7 +1131,10 @@
       <c r="E28" t="n">
         <v>220</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1070,7 +1156,10 @@
       <c r="E29" t="n">
         <v>230</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="n">
+        <v>9</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1092,7 +1181,10 @@
       <c r="E30" t="n">
         <v>234</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1114,7 +1206,10 @@
       <c r="E31" t="n">
         <v>236</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="n">
+        <v>8</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1136,7 +1231,10 @@
       <c r="E32" t="n">
         <v>244</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="n">
+        <v>6</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1158,7 +1256,10 @@
       <c r="E33" t="n">
         <v>125</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1180,7 +1281,10 @@
       <c r="E34" t="n">
         <v>93</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1202,7 +1306,10 @@
       <c r="E35" t="n">
         <v>360</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="n">
+        <v>15</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1224,7 +1331,10 @@
       <c r="E36" t="n">
         <v>260</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>14</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1246,7 +1356,10 @@
       <c r="E37" t="n">
         <v>158</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="n">
+        <v>6</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1268,7 +1381,10 @@
       <c r="E38" t="n">
         <v>130</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1290,7 +1406,10 @@
       <c r="E39" t="n">
         <v>103</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1312,7 +1431,10 @@
       <c r="E40" t="n">
         <v>118</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="n">
+        <v>3</v>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1334,7 +1456,10 @@
       <c r="E41" t="n">
         <v>126</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1356,7 +1481,10 @@
       <c r="E42" t="n">
         <v>151</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1378,7 +1506,10 @@
       <c r="E43" t="n">
         <v>367</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="n">
+        <v>15</v>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1400,7 +1531,10 @@
       <c r="E44" t="n">
         <v>266</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="n">
+        <v>6</v>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1422,7 +1556,10 @@
       <c r="E45" t="n">
         <v>188</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="n">
+        <v>9</v>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1444,7 +1581,10 @@
       <c r="E46" t="n">
         <v>141</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="n">
+        <v>8</v>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1466,7 +1606,10 @@
       <c r="E47" t="n">
         <v>111</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="n">
+        <v>11</v>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1488,7 +1631,10 @@
       <c r="E48" t="n">
         <v>131</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" t="n">
+        <v>10</v>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1510,7 +1656,10 @@
       <c r="E49" t="n">
         <v>98</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="n">
+        <v>6</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1532,7 +1681,10 @@
       <c r="E50" t="n">
         <v>138</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="n">
+        <v>10</v>
+      </c>
+      <c r="G50" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1554,7 +1706,10 @@
       <c r="E51" t="n">
         <v>154</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="n">
+        <v>16</v>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1576,7 +1731,10 @@
       <c r="E52" t="n">
         <v>224</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" t="n">
+        <v>13</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1598,7 +1756,10 @@
       <c r="E53" t="n">
         <v>273</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" t="n">
+        <v>12</v>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1620,7 +1781,10 @@
       <c r="E54" t="n">
         <v>301</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" t="n">
+        <v>17</v>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1642,7 +1806,10 @@
       <c r="E55" t="n">
         <v>239</v>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" t="n">
+        <v>9</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1664,7 +1831,10 @@
       <c r="E56" t="n">
         <v>216</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F56" t="n">
+        <v>12</v>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1686,7 +1856,10 @@
       <c r="E57" t="n">
         <v>154</v>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1708,7 +1881,10 @@
       <c r="E58" t="n">
         <v>107</v>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F58" t="n">
+        <v>6</v>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1730,7 +1906,10 @@
       <c r="E59" t="n">
         <v>219</v>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F59" t="n">
+        <v>3</v>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1752,7 +1931,10 @@
       <c r="E60" t="n">
         <v>151</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" t="n">
+        <v>5</v>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1774,7 +1956,10 @@
       <c r="E61" t="n">
         <v>151</v>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="F61" t="n">
+        <v>7</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1796,7 +1981,10 @@
       <c r="E62" t="n">
         <v>299</v>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="F62" t="n">
+        <v>13</v>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1818,7 +2006,10 @@
       <c r="E63" t="n">
         <v>250</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F63" t="n">
+        <v>15</v>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1840,7 +2031,10 @@
       <c r="E64" t="n">
         <v>214</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F64" t="n">
+        <v>13</v>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1862,7 +2056,10 @@
       <c r="E65" t="n">
         <v>132</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F65" t="n">
+        <v>5</v>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1884,7 +2081,10 @@
       <c r="E66" t="n">
         <v>128</v>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="F66" t="n">
+        <v>10</v>
+      </c>
+      <c r="G66" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1906,7 +2106,10 @@
       <c r="E67" t="n">
         <v>152</v>
       </c>
-      <c r="F67" t="inlineStr">
+      <c r="F67" t="n">
+        <v>11</v>
+      </c>
+      <c r="G67" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1928,7 +2131,10 @@
       <c r="E68" t="n">
         <v>240</v>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="F68" t="n">
+        <v>13</v>
+      </c>
+      <c r="G68" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1950,7 +2156,10 @@
       <c r="E69" t="n">
         <v>321</v>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="F69" t="n">
+        <v>6</v>
+      </c>
+      <c r="G69" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1972,7 +2181,10 @@
       <c r="E70" t="n">
         <v>229</v>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="F70" t="n">
+        <v>5</v>
+      </c>
+      <c r="G70" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1994,7 +2206,10 @@
       <c r="E71" t="n">
         <v>248</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="F71" t="n">
+        <v>6</v>
+      </c>
+      <c r="G71" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2016,7 +2231,10 @@
       <c r="E72" t="n">
         <v>213</v>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="F72" t="n">
+        <v>9</v>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2038,7 +2256,10 @@
       <c r="E73" t="n">
         <v>262</v>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F73" t="n">
+        <v>10</v>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2060,7 +2281,10 @@
       <c r="E74" t="n">
         <v>258</v>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="F74" t="n">
+        <v>3</v>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2082,7 +2306,10 @@
       <c r="E75" t="n">
         <v>239</v>
       </c>
-      <c r="F75" t="inlineStr">
+      <c r="F75" t="n">
+        <v>7</v>
+      </c>
+      <c r="G75" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2104,7 +2331,10 @@
       <c r="E76" t="n">
         <v>125</v>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F76" t="n">
+        <v>9</v>
+      </c>
+      <c r="G76" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2126,7 +2356,10 @@
       <c r="E77" t="n">
         <v>96</v>
       </c>
-      <c r="F77" t="inlineStr">
+      <c r="F77" t="n">
+        <v>5</v>
+      </c>
+      <c r="G77" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2148,7 +2381,10 @@
       <c r="E78" t="n">
         <v>159</v>
       </c>
-      <c r="F78" t="inlineStr">
+      <c r="F78" t="n">
+        <v>10</v>
+      </c>
+      <c r="G78" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2170,7 +2406,10 @@
       <c r="E79" t="n">
         <v>136</v>
       </c>
-      <c r="F79" t="inlineStr">
+      <c r="F79" t="n">
+        <v>4</v>
+      </c>
+      <c r="G79" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2192,7 +2431,10 @@
       <c r="E80" t="n">
         <v>94</v>
       </c>
-      <c r="F80" t="inlineStr">
+      <c r="F80" t="n">
+        <v>2</v>
+      </c>
+      <c r="G80" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2214,7 +2456,10 @@
       <c r="E81" t="n">
         <v>84</v>
       </c>
-      <c r="F81" t="inlineStr">
+      <c r="F81" t="n">
+        <v>2</v>
+      </c>
+      <c r="G81" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2236,7 +2481,10 @@
       <c r="E82" t="n">
         <v>108</v>
       </c>
-      <c r="F82" t="inlineStr">
+      <c r="F82" t="n">
+        <v>4</v>
+      </c>
+      <c r="G82" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2258,7 +2506,10 @@
       <c r="E83" t="n">
         <v>182</v>
       </c>
-      <c r="F83" t="inlineStr">
+      <c r="F83" t="n">
+        <v>5</v>
+      </c>
+      <c r="G83" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2280,7 +2531,10 @@
       <c r="E84" t="n">
         <v>77</v>
       </c>
-      <c r="F84" t="inlineStr">
+      <c r="F84" t="n">
+        <v>3</v>
+      </c>
+      <c r="G84" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2302,7 +2556,10 @@
       <c r="E85" t="n">
         <v>145</v>
       </c>
-      <c r="F85" t="inlineStr">
+      <c r="F85" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2324,7 +2581,10 @@
       <c r="E86" t="n">
         <v>139</v>
       </c>
-      <c r="F86" t="inlineStr">
+      <c r="F86" t="n">
+        <v>4</v>
+      </c>
+      <c r="G86" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2346,7 +2606,10 @@
       <c r="E87" t="n">
         <v>112</v>
       </c>
-      <c r="F87" t="inlineStr">
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2368,7 +2631,10 @@
       <c r="E88" t="n">
         <v>148</v>
       </c>
-      <c r="F88" t="inlineStr">
+      <c r="F88" t="n">
+        <v>4</v>
+      </c>
+      <c r="G88" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2390,7 +2656,10 @@
       <c r="E89" t="n">
         <v>111</v>
       </c>
-      <c r="F89" t="inlineStr">
+      <c r="F89" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2412,7 +2681,10 @@
       <c r="E90" t="n">
         <v>74</v>
       </c>
-      <c r="F90" t="inlineStr">
+      <c r="F90" t="n">
+        <v>5</v>
+      </c>
+      <c r="G90" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2434,7 +2706,10 @@
       <c r="E91" t="n">
         <v>58</v>
       </c>
-      <c r="F91" t="inlineStr">
+      <c r="F91" t="n">
+        <v>2</v>
+      </c>
+      <c r="G91" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2456,7 +2731,10 @@
       <c r="E92" t="n">
         <v>26</v>
       </c>
-      <c r="F92" t="inlineStr">
+      <c r="F92" t="n">
+        <v>1</v>
+      </c>
+      <c r="G92" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2478,7 +2756,10 @@
       <c r="E93" t="n">
         <v>117</v>
       </c>
-      <c r="F93" t="inlineStr">
+      <c r="F93" t="n">
+        <v>5</v>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2500,7 +2781,10 @@
       <c r="E94" t="n">
         <v>38</v>
       </c>
-      <c r="F94" t="inlineStr">
+      <c r="F94" t="n">
+        <v>5</v>
+      </c>
+      <c r="G94" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2522,7 +2806,10 @@
       <c r="E95" t="n">
         <v>151</v>
       </c>
-      <c r="F95" t="inlineStr">
+      <c r="F95" t="n">
+        <v>3</v>
+      </c>
+      <c r="G95" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2544,7 +2831,10 @@
       <c r="E96" t="n">
         <v>93</v>
       </c>
-      <c r="F96" t="inlineStr">
+      <c r="F96" t="n">
+        <v>5</v>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2566,7 +2856,10 @@
       <c r="E97" t="n">
         <v>76</v>
       </c>
-      <c r="F97" t="inlineStr">
+      <c r="F97" t="n">
+        <v>3</v>
+      </c>
+      <c r="G97" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2588,7 +2881,10 @@
       <c r="E98" t="n">
         <v>75</v>
       </c>
-      <c r="F98" t="inlineStr">
+      <c r="F98" t="n">
+        <v>3</v>
+      </c>
+      <c r="G98" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2610,7 +2906,10 @@
       <c r="E99" t="n">
         <v>87</v>
       </c>
-      <c r="F99" t="inlineStr">
+      <c r="F99" t="n">
+        <v>5</v>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2632,7 +2931,10 @@
       <c r="E100" t="n">
         <v>157</v>
       </c>
-      <c r="F100" t="inlineStr">
+      <c r="F100" t="n">
+        <v>3</v>
+      </c>
+      <c r="G100" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>

</xml_diff>

<commit_message>
Funktion für maximalen Histogrammwert in ImagePreprocessing implementiert
</commit_message>
<xml_diff>
--- a/Features_Test.xlsx
+++ b/Features_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>maximaler Histogrammwert</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Labels</t>
         </is>
       </c>
@@ -484,7 +489,10 @@
       <c r="F2" t="n">
         <v>3</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -509,7 +517,10 @@
       <c r="F3" t="n">
         <v>5</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>9953</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -534,7 +545,10 @@
       <c r="F4" t="n">
         <v>5</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>2449</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -559,7 +573,10 @@
       <c r="F5" t="n">
         <v>8</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="n">
+        <v>8822</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -584,7 +601,10 @@
       <c r="F6" t="n">
         <v>8</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="n">
+        <v>2264</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -609,7 +629,10 @@
       <c r="F7" t="n">
         <v>16</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="n">
+        <v>1875</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -634,7 +657,10 @@
       <c r="F8" t="n">
         <v>18</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" t="n">
+        <v>1663</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -659,7 +685,10 @@
       <c r="F9" t="n">
         <v>7</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" t="n">
+        <v>1667</v>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -684,7 +713,10 @@
       <c r="F10" t="n">
         <v>7</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" t="n">
+        <v>2512</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -709,7 +741,10 @@
       <c r="F11" t="n">
         <v>11</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="n">
+        <v>2513</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -734,7 +769,10 @@
       <c r="F12" t="n">
         <v>11</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="n">
+        <v>4969</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -759,7 +797,10 @@
       <c r="F13" t="n">
         <v>8</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>4667</v>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -784,7 +825,10 @@
       <c r="F14" t="n">
         <v>3</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="n">
+        <v>5133</v>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -809,7 +853,10 @@
       <c r="F15" t="n">
         <v>9</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="n">
+        <v>5561</v>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -834,7 +881,10 @@
       <c r="F16" t="n">
         <v>4</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="n">
+        <v>2372</v>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -859,7 +909,10 @@
       <c r="F17" t="n">
         <v>8</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" t="n">
+        <v>2657</v>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -884,7 +937,10 @@
       <c r="F18" t="n">
         <v>4</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="n">
+        <v>1741</v>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -909,7 +965,10 @@
       <c r="F19" t="n">
         <v>6</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="n">
+        <v>2943</v>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -934,7 +993,10 @@
       <c r="F20" t="n">
         <v>5</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="n">
+        <v>3181</v>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_geschlossen</t>
         </is>
@@ -959,7 +1021,10 @@
       <c r="F21" t="n">
         <v>7</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" t="n">
+        <v>5618</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -984,7 +1049,10 @@
       <c r="F22" t="n">
         <v>14</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" t="n">
+        <v>7165</v>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1009,7 +1077,10 @@
       <c r="F23" t="n">
         <v>12</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="n">
+        <v>6791</v>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1034,7 +1105,10 @@
       <c r="F24" t="n">
         <v>10</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="n">
+        <v>7682</v>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1059,7 +1133,10 @@
       <c r="F25" t="n">
         <v>11</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="n">
+        <v>7880</v>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1084,7 +1161,10 @@
       <c r="F26" t="n">
         <v>5</v>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" t="n">
+        <v>3401</v>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1109,7 +1189,10 @@
       <c r="F27" t="n">
         <v>5</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="n">
+        <v>3324</v>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1134,7 +1217,10 @@
       <c r="F28" t="n">
         <v>5</v>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="n">
+        <v>2283</v>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1159,7 +1245,10 @@
       <c r="F29" t="n">
         <v>9</v>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" t="n">
+        <v>2756</v>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1184,7 +1273,10 @@
       <c r="F30" t="n">
         <v>4</v>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="n">
+        <v>4375</v>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1209,7 +1301,10 @@
       <c r="F31" t="n">
         <v>8</v>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G31" t="n">
+        <v>1945</v>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1234,7 +1329,10 @@
       <c r="F32" t="n">
         <v>6</v>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="n">
+        <v>4170</v>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1259,7 +1357,10 @@
       <c r="F33" t="n">
         <v>4</v>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" t="n">
+        <v>3539</v>
+      </c>
+      <c r="H33" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1284,7 +1385,10 @@
       <c r="F34" t="n">
         <v>6</v>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="n">
+        <v>2024</v>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1309,7 +1413,10 @@
       <c r="F35" t="n">
         <v>15</v>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="n">
+        <v>1580</v>
+      </c>
+      <c r="H35" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1334,7 +1441,10 @@
       <c r="F36" t="n">
         <v>14</v>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" t="n">
+        <v>3077</v>
+      </c>
+      <c r="H36" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1359,7 +1469,10 @@
       <c r="F37" t="n">
         <v>6</v>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="G37" t="n">
+        <v>2976</v>
+      </c>
+      <c r="H37" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1384,7 +1497,10 @@
       <c r="F38" t="n">
         <v>6</v>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G38" t="n">
+        <v>2281</v>
+      </c>
+      <c r="H38" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1409,7 +1525,10 @@
       <c r="F39" t="n">
         <v>3</v>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="G39" t="n">
+        <v>3354</v>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1434,7 +1553,10 @@
       <c r="F40" t="n">
         <v>3</v>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G40" t="n">
+        <v>2684</v>
+      </c>
+      <c r="H40" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1459,7 +1581,10 @@
       <c r="F41" t="n">
         <v>5</v>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="G41" t="n">
+        <v>2321</v>
+      </c>
+      <c r="H41" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1484,7 +1609,10 @@
       <c r="F42" t="n">
         <v>8</v>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G42" t="n">
+        <v>2749</v>
+      </c>
+      <c r="H42" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1509,7 +1637,10 @@
       <c r="F43" t="n">
         <v>15</v>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="G43" t="n">
+        <v>2147</v>
+      </c>
+      <c r="H43" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1534,7 +1665,10 @@
       <c r="F44" t="n">
         <v>6</v>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G44" t="n">
+        <v>1510</v>
+      </c>
+      <c r="H44" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1559,7 +1693,10 @@
       <c r="F45" t="n">
         <v>9</v>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="G45" t="n">
+        <v>1246</v>
+      </c>
+      <c r="H45" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1584,7 +1721,10 @@
       <c r="F46" t="n">
         <v>8</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="n">
+        <v>2608</v>
+      </c>
+      <c r="H46" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1609,7 +1749,10 @@
       <c r="F47" t="n">
         <v>11</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="n">
+        <v>1652</v>
+      </c>
+      <c r="H47" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1634,7 +1777,10 @@
       <c r="F48" t="n">
         <v>10</v>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="n">
+        <v>7748</v>
+      </c>
+      <c r="H48" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1659,7 +1805,10 @@
       <c r="F49" t="n">
         <v>6</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>1686</v>
+      </c>
+      <c r="H49" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1684,7 +1833,10 @@
       <c r="F50" t="n">
         <v>10</v>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" t="n">
+        <v>1959</v>
+      </c>
+      <c r="H50" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1709,7 +1861,10 @@
       <c r="F51" t="n">
         <v>16</v>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G51" t="n">
+        <v>2158</v>
+      </c>
+      <c r="H51" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1734,7 +1889,10 @@
       <c r="F52" t="n">
         <v>13</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="n">
+        <v>1809</v>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1759,7 +1917,10 @@
       <c r="F53" t="n">
         <v>12</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" t="n">
+        <v>2255</v>
+      </c>
+      <c r="H53" t="inlineStr">
         <is>
           <t>Etikett_beschaedigt_Flasche_offen</t>
         </is>
@@ -1784,7 +1945,10 @@
       <c r="F54" t="n">
         <v>17</v>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G54" t="n">
+        <v>5691</v>
+      </c>
+      <c r="H54" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1809,7 +1973,10 @@
       <c r="F55" t="n">
         <v>9</v>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G55" t="n">
+        <v>841</v>
+      </c>
+      <c r="H55" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1834,7 +2001,10 @@
       <c r="F56" t="n">
         <v>12</v>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G56" t="n">
+        <v>1622</v>
+      </c>
+      <c r="H56" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1859,7 +2029,10 @@
       <c r="F57" t="n">
         <v>4</v>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G57" t="n">
+        <v>2343</v>
+      </c>
+      <c r="H57" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1884,7 +2057,10 @@
       <c r="F58" t="n">
         <v>6</v>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G58" t="n">
+        <v>2588</v>
+      </c>
+      <c r="H58" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1909,7 +2085,10 @@
       <c r="F59" t="n">
         <v>3</v>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="G59" t="n">
+        <v>1850</v>
+      </c>
+      <c r="H59" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1934,7 +2113,10 @@
       <c r="F60" t="n">
         <v>5</v>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="G60" t="n">
+        <v>1848</v>
+      </c>
+      <c r="H60" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1959,7 +2141,10 @@
       <c r="F61" t="n">
         <v>7</v>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="G61" t="n">
+        <v>1832</v>
+      </c>
+      <c r="H61" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -1984,7 +2169,10 @@
       <c r="F62" t="n">
         <v>13</v>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" t="n">
+        <v>4747</v>
+      </c>
+      <c r="H62" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2009,7 +2197,10 @@
       <c r="F63" t="n">
         <v>15</v>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="G63" t="n">
+        <v>4135</v>
+      </c>
+      <c r="H63" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2034,7 +2225,10 @@
       <c r="F64" t="n">
         <v>13</v>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="G64" t="n">
+        <v>2246</v>
+      </c>
+      <c r="H64" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2059,7 +2253,10 @@
       <c r="F65" t="n">
         <v>5</v>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="G65" t="n">
+        <v>2463</v>
+      </c>
+      <c r="H65" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2084,7 +2281,10 @@
       <c r="F66" t="n">
         <v>10</v>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="n">
+        <v>6457</v>
+      </c>
+      <c r="H66" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2109,7 +2309,10 @@
       <c r="F67" t="n">
         <v>11</v>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="G67" t="n">
+        <v>2268</v>
+      </c>
+      <c r="H67" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2134,7 +2337,10 @@
       <c r="F68" t="n">
         <v>13</v>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="G68" t="n">
+        <v>3411</v>
+      </c>
+      <c r="H68" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2159,7 +2365,10 @@
       <c r="F69" t="n">
         <v>6</v>
       </c>
-      <c r="G69" t="inlineStr">
+      <c r="G69" t="n">
+        <v>3820</v>
+      </c>
+      <c r="H69" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2184,7 +2393,10 @@
       <c r="F70" t="n">
         <v>5</v>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="n">
+        <v>4013</v>
+      </c>
+      <c r="H70" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2209,7 +2421,10 @@
       <c r="F71" t="n">
         <v>6</v>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" t="n">
+        <v>4168</v>
+      </c>
+      <c r="H71" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2234,7 +2449,10 @@
       <c r="F72" t="n">
         <v>9</v>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="G72" t="n">
+        <v>4165</v>
+      </c>
+      <c r="H72" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2259,7 +2477,10 @@
       <c r="F73" t="n">
         <v>10</v>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="G73" t="n">
+        <v>5732</v>
+      </c>
+      <c r="H73" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2284,7 +2505,10 @@
       <c r="F74" t="n">
         <v>3</v>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="G74" t="n">
+        <v>12524</v>
+      </c>
+      <c r="H74" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2309,7 +2533,10 @@
       <c r="F75" t="n">
         <v>7</v>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="n">
+        <v>11407</v>
+      </c>
+      <c r="H75" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2334,7 +2561,10 @@
       <c r="F76" t="n">
         <v>9</v>
       </c>
-      <c r="G76" t="inlineStr">
+      <c r="G76" t="n">
+        <v>3542</v>
+      </c>
+      <c r="H76" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2359,7 +2589,10 @@
       <c r="F77" t="n">
         <v>5</v>
       </c>
-      <c r="G77" t="inlineStr">
+      <c r="G77" t="n">
+        <v>2506</v>
+      </c>
+      <c r="H77" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2384,7 +2617,10 @@
       <c r="F78" t="n">
         <v>10</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>11423</v>
+      </c>
+      <c r="H78" t="inlineStr">
         <is>
           <t>Etikett_intakt_Flasche_geschlossen</t>
         </is>
@@ -2409,7 +2645,10 @@
       <c r="F79" t="n">
         <v>4</v>
       </c>
-      <c r="G79" t="inlineStr">
+      <c r="G79" t="n">
+        <v>2055</v>
+      </c>
+      <c r="H79" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2434,7 +2673,10 @@
       <c r="F80" t="n">
         <v>2</v>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="n">
+        <v>3541</v>
+      </c>
+      <c r="H80" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2459,7 +2701,10 @@
       <c r="F81" t="n">
         <v>2</v>
       </c>
-      <c r="G81" t="inlineStr">
+      <c r="G81" t="n">
+        <v>2600</v>
+      </c>
+      <c r="H81" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2484,7 +2729,10 @@
       <c r="F82" t="n">
         <v>4</v>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="G82" t="n">
+        <v>2288</v>
+      </c>
+      <c r="H82" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2509,7 +2757,10 @@
       <c r="F83" t="n">
         <v>5</v>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="G83" t="n">
+        <v>1468</v>
+      </c>
+      <c r="H83" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2534,7 +2785,10 @@
       <c r="F84" t="n">
         <v>3</v>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="G84" t="n">
+        <v>3334</v>
+      </c>
+      <c r="H84" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2559,7 +2813,10 @@
       <c r="F85" t="n">
         <v>1</v>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="G85" t="n">
+        <v>924</v>
+      </c>
+      <c r="H85" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2584,7 +2841,10 @@
       <c r="F86" t="n">
         <v>4</v>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="n">
+        <v>999</v>
+      </c>
+      <c r="H86" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2609,7 +2869,10 @@
       <c r="F87" t="n">
         <v>1</v>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="n">
+        <v>1518</v>
+      </c>
+      <c r="H87" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2634,7 +2897,10 @@
       <c r="F88" t="n">
         <v>4</v>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="n">
+        <v>955</v>
+      </c>
+      <c r="H88" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2659,7 +2925,10 @@
       <c r="F89" t="n">
         <v>1</v>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="n">
+        <v>1674</v>
+      </c>
+      <c r="H89" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2684,7 +2953,10 @@
       <c r="F90" t="n">
         <v>5</v>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="n">
+        <v>1606</v>
+      </c>
+      <c r="H90" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2709,7 +2981,10 @@
       <c r="F91" t="n">
         <v>2</v>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="n">
+        <v>2171</v>
+      </c>
+      <c r="H91" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2734,7 +3009,10 @@
       <c r="F92" t="n">
         <v>1</v>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="n">
+        <v>1213</v>
+      </c>
+      <c r="H92" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2759,7 +3037,10 @@
       <c r="F93" t="n">
         <v>5</v>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="n">
+        <v>2231</v>
+      </c>
+      <c r="H93" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2784,7 +3065,10 @@
       <c r="F94" t="n">
         <v>5</v>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="n">
+        <v>2682</v>
+      </c>
+      <c r="H94" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2809,7 +3093,10 @@
       <c r="F95" t="n">
         <v>3</v>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G95" t="n">
+        <v>3251</v>
+      </c>
+      <c r="H95" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2834,7 +3121,10 @@
       <c r="F96" t="n">
         <v>5</v>
       </c>
-      <c r="G96" t="inlineStr">
+      <c r="G96" t="n">
+        <v>3801</v>
+      </c>
+      <c r="H96" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2859,7 +3149,10 @@
       <c r="F97" t="n">
         <v>3</v>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="G97" t="n">
+        <v>2885</v>
+      </c>
+      <c r="H97" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2884,7 +3177,10 @@
       <c r="F98" t="n">
         <v>3</v>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="n">
+        <v>2363</v>
+      </c>
+      <c r="H98" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2909,7 +3205,10 @@
       <c r="F99" t="n">
         <v>5</v>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="n">
+        <v>2680</v>
+      </c>
+      <c r="H99" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>
@@ -2934,7 +3233,10 @@
       <c r="F100" t="n">
         <v>3</v>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="G100" t="n">
+        <v>5203</v>
+      </c>
+      <c r="H100" t="inlineStr">
         <is>
           <t>Flaschenhals_beschaedigt</t>
         </is>

</xml_diff>